<commit_message>
forgot to update failure log
</commit_message>
<xml_diff>
--- a/Part 4 - Failure Log.xlsx
+++ b/Part 4 - Failure Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Method</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Logging in with invalid user, do not create new account</t>
   </si>
   <si>
-    <t>Logging in with invalid user, create new account</t>
-  </si>
-  <si>
     <t>Logging in with valid user</t>
   </si>
   <si>
@@ -58,6 +55,15 @@
   </si>
   <si>
     <t>Modifying login() to accept an argument, the name of the file that contains the usernames.</t>
+  </si>
+  <si>
+    <t>Logging in with invalid user, create new FS account</t>
+  </si>
+  <si>
+    <t>Logging in with invalid user, create new RS account</t>
+  </si>
+  <si>
+    <t>Logging in with invalid user, create new PS account</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,13 +422,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -433,40 +439,62 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding coverage screenshots to failure log
</commit_message>
<xml_diff>
--- a/Part 4 - Failure Log.xlsx
+++ b/Part 4 - Failure Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Method</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Logging in with invalid user, create new PS account</t>
+  </si>
+  <si>
+    <t>Coverage stats</t>
   </si>
 </sst>
 </file>
@@ -113,6 +116,201 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304077</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104645</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6448425" y="209550"/>
+          <a:ext cx="5780952" cy="1038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342171</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="2476500"/>
+          <a:ext cx="5828571" cy="1019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>332649</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6448425" y="3638550"/>
+          <a:ext cx="5809524" cy="1019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323124</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="1333500"/>
+          <a:ext cx="5809524" cy="1019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>313600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6438900" y="5334000"/>
+          <a:ext cx="5800000" cy="1019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,91 +612,95 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E27" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
comments for branch and loop coverage
</commit_message>
<xml_diff>
--- a/Part 4 - Failure Log.xlsx
+++ b/Part 4 - Failure Log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjgau\Documents\GitHub\lab1\OT-Bnb\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AEDAE0-7D8A-4E94-A50A-81A1BDEE5B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1080" windowWidth="43200" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="1080" windowWidth="29040" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,7 +181,7 @@
         <xdr:cNvPr id="2" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -221,7 +215,7 @@
         <xdr:cNvPr id="3" name="image5.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -255,7 +249,7 @@
         <xdr:cNvPr id="4" name="image3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -289,7 +283,7 @@
         <xdr:cNvPr id="5" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -323,7 +317,7 @@
         <xdr:cNvPr id="6" name="image8.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -357,7 +351,7 @@
         <xdr:cNvPr id="7" name="image1.png" title="Image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -391,7 +385,7 @@
         <xdr:cNvPr id="8" name="image6.png" title="Image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -425,7 +419,7 @@
         <xdr:cNvPr id="9" name="image7.png" title="Image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -464,7 +458,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16772DB6-46D0-4C72-9039-8631788FBC94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16772DB6-46D0-4C72-9039-8631788FBC94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -508,7 +502,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CAB8014-C608-4DE6-A13A-856B0291BF8B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5CAB8014-C608-4DE6-A13A-856B0291BF8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -552,7 +546,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A00EA539-6472-4AE4-8F3D-046D60E7FB71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A00EA539-6472-4AE4-8F3D-046D60E7FB71}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -778,10 +772,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
@@ -1933,7 +1927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2930,7 +2924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>